<commit_message>
Actualizar consumo_real.xlsx con nuevos datos
</commit_message>
<xml_diff>
--- a/distances_26-11 al 03-12.xlsx
+++ b/distances_26-11 al 03-12.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Periodo 26-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\consumo-bca-dashboard-limpio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BB7E36-F576-458B-8360-ED156ECB1FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4AF41B-5094-4C97-8615-0C005E52FBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="670">
   <si>
     <t>Grupo</t>
   </si>
@@ -2468,10 +2468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K324"/>
+  <dimension ref="A1:K433"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C205" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="H325" sqref="H325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13829,17 +13829,3511 @@
         <v>14</v>
       </c>
     </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>11</v>
+      </c>
+      <c r="B325" t="s">
+        <v>12</v>
+      </c>
+      <c r="C325" t="s">
+        <v>13</v>
+      </c>
+      <c r="D325" t="s">
+        <v>14</v>
+      </c>
+      <c r="E325" t="s">
+        <v>15</v>
+      </c>
+      <c r="F325" t="s">
+        <v>14</v>
+      </c>
+      <c r="G325" t="s">
+        <v>14</v>
+      </c>
+      <c r="H325" t="s">
+        <v>558</v>
+      </c>
+      <c r="I325">
+        <v>16</v>
+      </c>
+      <c r="J325">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>11</v>
+      </c>
+      <c r="B326" t="s">
+        <v>17</v>
+      </c>
+      <c r="C326" t="s">
+        <v>18</v>
+      </c>
+      <c r="D326" t="s">
+        <v>14</v>
+      </c>
+      <c r="E326" t="s">
+        <v>19</v>
+      </c>
+      <c r="F326" t="s">
+        <v>14</v>
+      </c>
+      <c r="G326" t="s">
+        <v>14</v>
+      </c>
+      <c r="H326" t="s">
+        <v>559</v>
+      </c>
+      <c r="I326">
+        <v>8</v>
+      </c>
+      <c r="J326">
+        <v>2197.5300000000002</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>11</v>
+      </c>
+      <c r="B327" t="s">
+        <v>560</v>
+      </c>
+      <c r="C327" t="s">
+        <v>22</v>
+      </c>
+      <c r="D327" t="s">
+        <v>14</v>
+      </c>
+      <c r="E327" t="s">
+        <v>23</v>
+      </c>
+      <c r="F327" t="s">
+        <v>14</v>
+      </c>
+      <c r="G327" t="s">
+        <v>14</v>
+      </c>
+      <c r="H327" t="s">
+        <v>561</v>
+      </c>
+      <c r="I327">
+        <v>12</v>
+      </c>
+      <c r="J327">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>11</v>
+      </c>
+      <c r="B328" t="s">
+        <v>25</v>
+      </c>
+      <c r="C328" t="s">
+        <v>26</v>
+      </c>
+      <c r="D328" t="s">
+        <v>14</v>
+      </c>
+      <c r="E328" t="s">
+        <v>27</v>
+      </c>
+      <c r="F328" t="s">
+        <v>14</v>
+      </c>
+      <c r="G328" t="s">
+        <v>14</v>
+      </c>
+      <c r="H328" t="s">
+        <v>562</v>
+      </c>
+      <c r="I328">
+        <v>15</v>
+      </c>
+      <c r="J328">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>11</v>
+      </c>
+      <c r="B329" t="s">
+        <v>29</v>
+      </c>
+      <c r="C329" t="s">
+        <v>30</v>
+      </c>
+      <c r="D329" t="s">
+        <v>14</v>
+      </c>
+      <c r="E329" t="s">
+        <v>31</v>
+      </c>
+      <c r="F329" t="s">
+        <v>14</v>
+      </c>
+      <c r="G329" t="s">
+        <v>14</v>
+      </c>
+      <c r="H329" t="s">
+        <v>563</v>
+      </c>
+      <c r="I329">
+        <v>18</v>
+      </c>
+      <c r="J329">
+        <v>1442.76</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>11</v>
+      </c>
+      <c r="B330" t="s">
+        <v>33</v>
+      </c>
+      <c r="C330" t="s">
+        <v>34</v>
+      </c>
+      <c r="D330" t="s">
+        <v>14</v>
+      </c>
+      <c r="E330" t="s">
+        <v>35</v>
+      </c>
+      <c r="F330" t="s">
+        <v>14</v>
+      </c>
+      <c r="G330" t="s">
+        <v>14</v>
+      </c>
+      <c r="H330" t="s">
+        <v>564</v>
+      </c>
+      <c r="I330">
+        <v>4</v>
+      </c>
+      <c r="J330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>11</v>
+      </c>
+      <c r="B331" t="s">
+        <v>37</v>
+      </c>
+      <c r="C331" t="s">
+        <v>38</v>
+      </c>
+      <c r="D331" t="s">
+        <v>14</v>
+      </c>
+      <c r="E331" t="s">
+        <v>39</v>
+      </c>
+      <c r="F331" t="s">
+        <v>14</v>
+      </c>
+      <c r="G331" t="s">
+        <v>14</v>
+      </c>
+      <c r="H331" t="s">
+        <v>565</v>
+      </c>
+      <c r="I331">
+        <v>10</v>
+      </c>
+      <c r="J331">
+        <v>451.5</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>11</v>
+      </c>
+      <c r="B332" t="s">
+        <v>41</v>
+      </c>
+      <c r="C332" t="s">
+        <v>42</v>
+      </c>
+      <c r="D332" t="s">
+        <v>14</v>
+      </c>
+      <c r="E332" t="s">
+        <v>43</v>
+      </c>
+      <c r="F332" t="s">
+        <v>14</v>
+      </c>
+      <c r="G332" t="s">
+        <v>14</v>
+      </c>
+      <c r="H332" t="s">
+        <v>566</v>
+      </c>
+      <c r="I332">
+        <v>15</v>
+      </c>
+      <c r="J332">
+        <v>2372.1799999999998</v>
+      </c>
+    </row>
+    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>11</v>
+      </c>
+      <c r="B333" t="s">
+        <v>45</v>
+      </c>
+      <c r="C333" t="s">
+        <v>46</v>
+      </c>
+      <c r="D333" t="s">
+        <v>14</v>
+      </c>
+      <c r="E333" t="s">
+        <v>47</v>
+      </c>
+      <c r="F333" t="s">
+        <v>14</v>
+      </c>
+      <c r="G333" t="s">
+        <v>14</v>
+      </c>
+      <c r="H333" t="s">
+        <v>567</v>
+      </c>
+      <c r="I333">
+        <v>17</v>
+      </c>
+      <c r="J333">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>11</v>
+      </c>
+      <c r="B334" t="s">
+        <v>49</v>
+      </c>
+      <c r="C334" t="s">
+        <v>50</v>
+      </c>
+      <c r="D334" t="s">
+        <v>14</v>
+      </c>
+      <c r="E334" t="s">
+        <v>51</v>
+      </c>
+      <c r="F334" t="s">
+        <v>14</v>
+      </c>
+      <c r="G334" t="s">
+        <v>14</v>
+      </c>
+      <c r="H334" t="s">
+        <v>568</v>
+      </c>
+      <c r="I334">
+        <v>17</v>
+      </c>
+      <c r="J334">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>11</v>
+      </c>
+      <c r="B335" t="s">
+        <v>53</v>
+      </c>
+      <c r="C335" t="s">
+        <v>54</v>
+      </c>
+      <c r="D335" t="s">
+        <v>14</v>
+      </c>
+      <c r="E335" t="s">
+        <v>55</v>
+      </c>
+      <c r="F335" t="s">
+        <v>14</v>
+      </c>
+      <c r="G335" t="s">
+        <v>14</v>
+      </c>
+      <c r="H335" t="s">
+        <v>569</v>
+      </c>
+      <c r="I335">
+        <v>13</v>
+      </c>
+      <c r="J335">
+        <v>3751.85</v>
+      </c>
+    </row>
+    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>11</v>
+      </c>
+      <c r="B336" t="s">
+        <v>57</v>
+      </c>
+      <c r="C336" t="s">
+        <v>58</v>
+      </c>
+      <c r="D336" t="s">
+        <v>14</v>
+      </c>
+      <c r="E336" t="s">
+        <v>59</v>
+      </c>
+      <c r="F336" t="s">
+        <v>14</v>
+      </c>
+      <c r="G336" t="s">
+        <v>14</v>
+      </c>
+      <c r="H336" t="s">
+        <v>570</v>
+      </c>
+      <c r="I336">
+        <v>12</v>
+      </c>
+      <c r="J336">
+        <v>3835.06</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>11</v>
+      </c>
+      <c r="B337" t="s">
+        <v>61</v>
+      </c>
+      <c r="C337" t="s">
+        <v>62</v>
+      </c>
+      <c r="D337" t="s">
+        <v>14</v>
+      </c>
+      <c r="E337" t="s">
+        <v>63</v>
+      </c>
+      <c r="F337" t="s">
+        <v>14</v>
+      </c>
+      <c r="G337" t="s">
+        <v>14</v>
+      </c>
+      <c r="H337" t="s">
+        <v>571</v>
+      </c>
+      <c r="I337">
+        <v>16</v>
+      </c>
+      <c r="J337">
+        <v>3166.69</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>11</v>
+      </c>
+      <c r="B338" t="s">
+        <v>65</v>
+      </c>
+      <c r="C338" t="s">
+        <v>66</v>
+      </c>
+      <c r="D338" t="s">
+        <v>14</v>
+      </c>
+      <c r="E338" t="s">
+        <v>67</v>
+      </c>
+      <c r="F338" t="s">
+        <v>14</v>
+      </c>
+      <c r="G338" t="s">
+        <v>14</v>
+      </c>
+      <c r="H338" t="s">
+        <v>572</v>
+      </c>
+      <c r="I338">
+        <v>13</v>
+      </c>
+      <c r="J338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>11</v>
+      </c>
+      <c r="B339" t="s">
+        <v>471</v>
+      </c>
+      <c r="C339" t="s">
+        <v>70</v>
+      </c>
+      <c r="D339" t="s">
+        <v>14</v>
+      </c>
+      <c r="E339" t="s">
+        <v>71</v>
+      </c>
+      <c r="F339" t="s">
+        <v>14</v>
+      </c>
+      <c r="G339" t="s">
+        <v>14</v>
+      </c>
+      <c r="H339" t="s">
+        <v>573</v>
+      </c>
+      <c r="I339">
+        <v>16</v>
+      </c>
+      <c r="J339">
+        <v>3634</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>11</v>
+      </c>
+      <c r="B340" t="s">
+        <v>73</v>
+      </c>
+      <c r="C340" t="s">
+        <v>74</v>
+      </c>
+      <c r="D340" t="s">
+        <v>14</v>
+      </c>
+      <c r="E340" t="s">
+        <v>75</v>
+      </c>
+      <c r="F340" t="s">
+        <v>14</v>
+      </c>
+      <c r="G340" t="s">
+        <v>14</v>
+      </c>
+      <c r="H340" t="s">
+        <v>574</v>
+      </c>
+      <c r="I340">
+        <v>13</v>
+      </c>
+      <c r="J340">
+        <v>2438.5</v>
+      </c>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>11</v>
+      </c>
+      <c r="B341" t="s">
+        <v>77</v>
+      </c>
+      <c r="C341" t="s">
+        <v>78</v>
+      </c>
+      <c r="D341" t="s">
+        <v>14</v>
+      </c>
+      <c r="E341" t="s">
+        <v>79</v>
+      </c>
+      <c r="F341" t="s">
+        <v>14</v>
+      </c>
+      <c r="G341" t="s">
+        <v>14</v>
+      </c>
+      <c r="H341" t="s">
+        <v>575</v>
+      </c>
+      <c r="I341">
+        <v>7</v>
+      </c>
+      <c r="J341">
+        <v>1467.13</v>
+      </c>
+    </row>
+    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>11</v>
+      </c>
+      <c r="B342" t="s">
+        <v>475</v>
+      </c>
+      <c r="C342" t="s">
+        <v>82</v>
+      </c>
+      <c r="D342" t="s">
+        <v>14</v>
+      </c>
+      <c r="E342" t="s">
+        <v>83</v>
+      </c>
+      <c r="F342" t="s">
+        <v>14</v>
+      </c>
+      <c r="G342" t="s">
+        <v>14</v>
+      </c>
+      <c r="H342" t="s">
+        <v>576</v>
+      </c>
+      <c r="I342">
+        <v>9</v>
+      </c>
+      <c r="J342">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>11</v>
+      </c>
+      <c r="B343" t="s">
+        <v>85</v>
+      </c>
+      <c r="C343" t="s">
+        <v>86</v>
+      </c>
+      <c r="D343" t="s">
+        <v>14</v>
+      </c>
+      <c r="E343" t="s">
+        <v>87</v>
+      </c>
+      <c r="F343" t="s">
+        <v>14</v>
+      </c>
+      <c r="G343" t="s">
+        <v>14</v>
+      </c>
+      <c r="H343" t="s">
+        <v>577</v>
+      </c>
+      <c r="I343">
+        <v>13</v>
+      </c>
+      <c r="J343">
+        <v>3243.79</v>
+      </c>
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>11</v>
+      </c>
+      <c r="B344" t="s">
+        <v>578</v>
+      </c>
+      <c r="C344" t="s">
+        <v>90</v>
+      </c>
+      <c r="D344" t="s">
+        <v>14</v>
+      </c>
+      <c r="E344" t="s">
+        <v>91</v>
+      </c>
+      <c r="F344" t="s">
+        <v>14</v>
+      </c>
+      <c r="G344" t="s">
+        <v>14</v>
+      </c>
+      <c r="H344" t="s">
+        <v>579</v>
+      </c>
+      <c r="I344">
+        <v>16</v>
+      </c>
+      <c r="J344">
+        <v>2715.51</v>
+      </c>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>11</v>
+      </c>
+      <c r="B345" t="s">
+        <v>93</v>
+      </c>
+      <c r="C345" t="s">
+        <v>94</v>
+      </c>
+      <c r="D345" t="s">
+        <v>14</v>
+      </c>
+      <c r="E345" t="s">
+        <v>95</v>
+      </c>
+      <c r="F345" t="s">
+        <v>14</v>
+      </c>
+      <c r="G345" t="s">
+        <v>14</v>
+      </c>
+      <c r="H345" t="s">
+        <v>580</v>
+      </c>
+      <c r="I345">
+        <v>22</v>
+      </c>
+      <c r="J345">
+        <v>3076</v>
+      </c>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>11</v>
+      </c>
+      <c r="B346" t="s">
+        <v>100</v>
+      </c>
+      <c r="C346" t="s">
+        <v>101</v>
+      </c>
+      <c r="D346" t="s">
+        <v>14</v>
+      </c>
+      <c r="E346" t="s">
+        <v>102</v>
+      </c>
+      <c r="F346" t="s">
+        <v>14</v>
+      </c>
+      <c r="G346" t="s">
+        <v>14</v>
+      </c>
+      <c r="H346" t="s">
+        <v>581</v>
+      </c>
+      <c r="I346">
+        <v>15</v>
+      </c>
+      <c r="J346">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>11</v>
+      </c>
+      <c r="B347" t="s">
+        <v>104</v>
+      </c>
+      <c r="C347" t="s">
+        <v>105</v>
+      </c>
+      <c r="D347" t="s">
+        <v>14</v>
+      </c>
+      <c r="E347" t="s">
+        <v>106</v>
+      </c>
+      <c r="F347" t="s">
+        <v>14</v>
+      </c>
+      <c r="G347" t="s">
+        <v>14</v>
+      </c>
+      <c r="H347" t="s">
+        <v>582</v>
+      </c>
+      <c r="I347">
+        <v>16</v>
+      </c>
+      <c r="J347">
+        <v>1827.51</v>
+      </c>
+    </row>
+    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>11</v>
+      </c>
+      <c r="B348" t="s">
+        <v>583</v>
+      </c>
+      <c r="C348" t="s">
+        <v>109</v>
+      </c>
+      <c r="D348" t="s">
+        <v>14</v>
+      </c>
+      <c r="E348" t="s">
+        <v>110</v>
+      </c>
+      <c r="F348" t="s">
+        <v>14</v>
+      </c>
+      <c r="G348" t="s">
+        <v>14</v>
+      </c>
+      <c r="H348" t="s">
+        <v>584</v>
+      </c>
+      <c r="I348">
+        <v>16</v>
+      </c>
+      <c r="J348">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>11</v>
+      </c>
+      <c r="B349" t="s">
+        <v>112</v>
+      </c>
+      <c r="C349" t="s">
+        <v>113</v>
+      </c>
+      <c r="D349" t="s">
+        <v>14</v>
+      </c>
+      <c r="E349" t="s">
+        <v>114</v>
+      </c>
+      <c r="F349" t="s">
+        <v>14</v>
+      </c>
+      <c r="G349" t="s">
+        <v>14</v>
+      </c>
+      <c r="H349" t="s">
+        <v>585</v>
+      </c>
+      <c r="I349">
+        <v>22</v>
+      </c>
+      <c r="J349">
+        <v>2905.76</v>
+      </c>
+    </row>
+    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>11</v>
+      </c>
+      <c r="B350" t="s">
+        <v>117</v>
+      </c>
+      <c r="C350" t="s">
+        <v>117</v>
+      </c>
+      <c r="D350" t="s">
+        <v>14</v>
+      </c>
+      <c r="E350" t="s">
+        <v>118</v>
+      </c>
+      <c r="F350" t="s">
+        <v>14</v>
+      </c>
+      <c r="G350" t="s">
+        <v>14</v>
+      </c>
+      <c r="H350" t="s">
+        <v>586</v>
+      </c>
+      <c r="I350">
+        <v>8</v>
+      </c>
+      <c r="J350">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>11</v>
+      </c>
+      <c r="B351" t="s">
+        <v>120</v>
+      </c>
+      <c r="C351" t="s">
+        <v>121</v>
+      </c>
+      <c r="D351" t="s">
+        <v>14</v>
+      </c>
+      <c r="E351" t="s">
+        <v>122</v>
+      </c>
+      <c r="F351" t="s">
+        <v>14</v>
+      </c>
+      <c r="G351" t="s">
+        <v>14</v>
+      </c>
+      <c r="H351" t="s">
+        <v>587</v>
+      </c>
+      <c r="I351">
+        <v>16</v>
+      </c>
+      <c r="J351">
+        <v>3458</v>
+      </c>
+    </row>
+    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>11</v>
+      </c>
+      <c r="B352" t="s">
+        <v>124</v>
+      </c>
+      <c r="C352" t="s">
+        <v>125</v>
+      </c>
+      <c r="D352" t="s">
+        <v>14</v>
+      </c>
+      <c r="E352" t="s">
+        <v>126</v>
+      </c>
+      <c r="F352" t="s">
+        <v>14</v>
+      </c>
+      <c r="G352" t="s">
+        <v>14</v>
+      </c>
+      <c r="H352" t="s">
+        <v>485</v>
+      </c>
+      <c r="I352">
+        <v>1</v>
+      </c>
+      <c r="J352">
+        <v>261.75</v>
+      </c>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>11</v>
+      </c>
+      <c r="B353" t="s">
+        <v>128</v>
+      </c>
+      <c r="C353" t="s">
+        <v>129</v>
+      </c>
+      <c r="D353" t="s">
+        <v>14</v>
+      </c>
+      <c r="E353" t="s">
+        <v>130</v>
+      </c>
+      <c r="F353" t="s">
+        <v>14</v>
+      </c>
+      <c r="G353" t="s">
+        <v>14</v>
+      </c>
+      <c r="H353" t="s">
+        <v>588</v>
+      </c>
+      <c r="I353">
+        <v>20</v>
+      </c>
+      <c r="J353">
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="354" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>11</v>
+      </c>
+      <c r="B354" t="s">
+        <v>132</v>
+      </c>
+      <c r="C354" t="s">
+        <v>132</v>
+      </c>
+      <c r="D354" t="s">
+        <v>14</v>
+      </c>
+      <c r="E354" t="s">
+        <v>133</v>
+      </c>
+      <c r="F354" t="s">
+        <v>14</v>
+      </c>
+      <c r="G354" t="s">
+        <v>14</v>
+      </c>
+      <c r="H354" t="s">
+        <v>487</v>
+      </c>
+      <c r="I354">
+        <v>1</v>
+      </c>
+      <c r="J354">
+        <v>155.69</v>
+      </c>
+    </row>
+    <row r="355" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>11</v>
+      </c>
+      <c r="B355" t="s">
+        <v>135</v>
+      </c>
+      <c r="C355" t="s">
+        <v>136</v>
+      </c>
+      <c r="D355" t="s">
+        <v>14</v>
+      </c>
+      <c r="E355" t="s">
+        <v>137</v>
+      </c>
+      <c r="F355" t="s">
+        <v>14</v>
+      </c>
+      <c r="G355" t="s">
+        <v>14</v>
+      </c>
+      <c r="H355" t="s">
+        <v>589</v>
+      </c>
+      <c r="I355">
+        <v>14</v>
+      </c>
+      <c r="J355">
+        <v>2795</v>
+      </c>
+    </row>
+    <row r="356" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>11</v>
+      </c>
+      <c r="B356" t="s">
+        <v>139</v>
+      </c>
+      <c r="C356" t="s">
+        <v>140</v>
+      </c>
+      <c r="D356" t="s">
+        <v>14</v>
+      </c>
+      <c r="E356" t="s">
+        <v>141</v>
+      </c>
+      <c r="F356" t="s">
+        <v>14</v>
+      </c>
+      <c r="G356" t="s">
+        <v>14</v>
+      </c>
+      <c r="H356" t="s">
+        <v>590</v>
+      </c>
+      <c r="I356">
+        <v>4</v>
+      </c>
+      <c r="J356">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="357" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>11</v>
+      </c>
+      <c r="B357" t="s">
+        <v>143</v>
+      </c>
+      <c r="C357" t="s">
+        <v>144</v>
+      </c>
+      <c r="D357" t="s">
+        <v>14</v>
+      </c>
+      <c r="E357" t="s">
+        <v>145</v>
+      </c>
+      <c r="F357" t="s">
+        <v>14</v>
+      </c>
+      <c r="G357" t="s">
+        <v>14</v>
+      </c>
+      <c r="H357" t="s">
+        <v>591</v>
+      </c>
+      <c r="I357">
+        <v>14</v>
+      </c>
+      <c r="J357">
+        <v>270305.42</v>
+      </c>
+    </row>
+    <row r="358" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>11</v>
+      </c>
+      <c r="B358" t="s">
+        <v>592</v>
+      </c>
+      <c r="C358" t="s">
+        <v>148</v>
+      </c>
+      <c r="D358" t="s">
+        <v>14</v>
+      </c>
+      <c r="E358" t="s">
+        <v>149</v>
+      </c>
+      <c r="F358" t="s">
+        <v>14</v>
+      </c>
+      <c r="G358" t="s">
+        <v>14</v>
+      </c>
+      <c r="H358" t="s">
+        <v>593</v>
+      </c>
+      <c r="I358">
+        <v>15</v>
+      </c>
+      <c r="J358">
+        <v>1563.56</v>
+      </c>
+    </row>
+    <row r="359" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>11</v>
+      </c>
+      <c r="B359" t="s">
+        <v>151</v>
+      </c>
+      <c r="C359" t="s">
+        <v>152</v>
+      </c>
+      <c r="D359" t="s">
+        <v>14</v>
+      </c>
+      <c r="E359" t="s">
+        <v>153</v>
+      </c>
+      <c r="F359" t="s">
+        <v>14</v>
+      </c>
+      <c r="G359" t="s">
+        <v>14</v>
+      </c>
+      <c r="H359" t="s">
+        <v>594</v>
+      </c>
+      <c r="I359">
+        <v>21</v>
+      </c>
+      <c r="J359">
+        <v>3654.22</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>11</v>
+      </c>
+      <c r="B360" t="s">
+        <v>595</v>
+      </c>
+      <c r="C360" t="s">
+        <v>156</v>
+      </c>
+      <c r="D360" t="s">
+        <v>14</v>
+      </c>
+      <c r="E360" t="s">
+        <v>157</v>
+      </c>
+      <c r="F360" t="s">
+        <v>14</v>
+      </c>
+      <c r="G360" t="s">
+        <v>14</v>
+      </c>
+      <c r="H360" t="s">
+        <v>596</v>
+      </c>
+      <c r="I360">
+        <v>12</v>
+      </c>
+      <c r="J360">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="361" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>11</v>
+      </c>
+      <c r="B361" t="s">
+        <v>159</v>
+      </c>
+      <c r="C361" t="s">
+        <v>160</v>
+      </c>
+      <c r="D361" t="s">
+        <v>14</v>
+      </c>
+      <c r="E361" t="s">
+        <v>161</v>
+      </c>
+      <c r="F361" t="s">
+        <v>14</v>
+      </c>
+      <c r="G361" t="s">
+        <v>14</v>
+      </c>
+      <c r="H361" t="s">
+        <v>597</v>
+      </c>
+      <c r="I361">
+        <v>13</v>
+      </c>
+      <c r="J361">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>11</v>
+      </c>
+      <c r="B362" t="s">
+        <v>163</v>
+      </c>
+      <c r="C362" t="s">
+        <v>164</v>
+      </c>
+      <c r="D362" t="s">
+        <v>14</v>
+      </c>
+      <c r="E362" t="s">
+        <v>165</v>
+      </c>
+      <c r="F362" t="s">
+        <v>14</v>
+      </c>
+      <c r="G362" t="s">
+        <v>14</v>
+      </c>
+      <c r="H362" t="s">
+        <v>598</v>
+      </c>
+      <c r="I362">
+        <v>13</v>
+      </c>
+      <c r="J362">
+        <v>2614.0700000000002</v>
+      </c>
+    </row>
+    <row r="363" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>11</v>
+      </c>
+      <c r="B363" t="s">
+        <v>167</v>
+      </c>
+      <c r="C363" t="s">
+        <v>168</v>
+      </c>
+      <c r="D363" t="s">
+        <v>14</v>
+      </c>
+      <c r="E363" t="s">
+        <v>169</v>
+      </c>
+      <c r="F363" t="s">
+        <v>14</v>
+      </c>
+      <c r="G363" t="s">
+        <v>14</v>
+      </c>
+      <c r="H363" t="s">
+        <v>599</v>
+      </c>
+      <c r="I363">
+        <v>11</v>
+      </c>
+      <c r="J363">
+        <v>3126.15</v>
+      </c>
+    </row>
+    <row r="364" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>11</v>
+      </c>
+      <c r="B364" t="s">
+        <v>171</v>
+      </c>
+      <c r="C364" t="s">
+        <v>172</v>
+      </c>
+      <c r="D364" t="s">
+        <v>14</v>
+      </c>
+      <c r="E364" t="s">
+        <v>173</v>
+      </c>
+      <c r="F364" t="s">
+        <v>14</v>
+      </c>
+      <c r="G364" t="s">
+        <v>14</v>
+      </c>
+      <c r="H364" t="s">
+        <v>497</v>
+      </c>
+      <c r="I364">
+        <v>2</v>
+      </c>
+      <c r="J364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>11</v>
+      </c>
+      <c r="B365" t="s">
+        <v>175</v>
+      </c>
+      <c r="C365" t="s">
+        <v>176</v>
+      </c>
+      <c r="D365" t="s">
+        <v>14</v>
+      </c>
+      <c r="E365" t="s">
+        <v>177</v>
+      </c>
+      <c r="F365" t="s">
+        <v>14</v>
+      </c>
+      <c r="G365" t="s">
+        <v>14</v>
+      </c>
+      <c r="H365" t="s">
+        <v>600</v>
+      </c>
+      <c r="I365">
+        <v>11</v>
+      </c>
+      <c r="J365">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>11</v>
+      </c>
+      <c r="B366" t="s">
+        <v>179</v>
+      </c>
+      <c r="C366" t="s">
+        <v>180</v>
+      </c>
+      <c r="D366" t="s">
+        <v>14</v>
+      </c>
+      <c r="E366" t="s">
+        <v>181</v>
+      </c>
+      <c r="F366" t="s">
+        <v>14</v>
+      </c>
+      <c r="G366" t="s">
+        <v>14</v>
+      </c>
+      <c r="H366" t="s">
+        <v>601</v>
+      </c>
+      <c r="I366">
+        <v>17</v>
+      </c>
+      <c r="J366">
+        <v>2615.44</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>11</v>
+      </c>
+      <c r="B367" t="s">
+        <v>183</v>
+      </c>
+      <c r="C367" t="s">
+        <v>184</v>
+      </c>
+      <c r="D367" t="s">
+        <v>14</v>
+      </c>
+      <c r="E367" t="s">
+        <v>185</v>
+      </c>
+      <c r="F367" t="s">
+        <v>14</v>
+      </c>
+      <c r="G367" t="s">
+        <v>14</v>
+      </c>
+      <c r="H367" t="s">
+        <v>602</v>
+      </c>
+      <c r="I367">
+        <v>12</v>
+      </c>
+      <c r="J367">
+        <v>3032.94</v>
+      </c>
+    </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>11</v>
+      </c>
+      <c r="B368" t="s">
+        <v>187</v>
+      </c>
+      <c r="C368" t="s">
+        <v>188</v>
+      </c>
+      <c r="D368" t="s">
+        <v>14</v>
+      </c>
+      <c r="E368" t="s">
+        <v>189</v>
+      </c>
+      <c r="F368" t="s">
+        <v>14</v>
+      </c>
+      <c r="G368" t="s">
+        <v>14</v>
+      </c>
+      <c r="H368" t="s">
+        <v>603</v>
+      </c>
+      <c r="I368">
+        <v>22</v>
+      </c>
+      <c r="J368">
+        <v>3290.76</v>
+      </c>
+    </row>
+    <row r="369" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>11</v>
+      </c>
+      <c r="B369" t="s">
+        <v>191</v>
+      </c>
+      <c r="C369" t="s">
+        <v>192</v>
+      </c>
+      <c r="D369" t="s">
+        <v>14</v>
+      </c>
+      <c r="E369" t="s">
+        <v>193</v>
+      </c>
+      <c r="F369" t="s">
+        <v>14</v>
+      </c>
+      <c r="G369" t="s">
+        <v>14</v>
+      </c>
+      <c r="H369" t="s">
+        <v>604</v>
+      </c>
+      <c r="I369">
+        <v>17</v>
+      </c>
+      <c r="J369">
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="370" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>11</v>
+      </c>
+      <c r="B370" t="s">
+        <v>195</v>
+      </c>
+      <c r="C370" t="s">
+        <v>196</v>
+      </c>
+      <c r="D370" t="s">
+        <v>14</v>
+      </c>
+      <c r="E370" t="s">
+        <v>197</v>
+      </c>
+      <c r="F370" t="s">
+        <v>14</v>
+      </c>
+      <c r="G370" t="s">
+        <v>14</v>
+      </c>
+      <c r="H370" t="s">
+        <v>605</v>
+      </c>
+      <c r="I370">
+        <v>14</v>
+      </c>
+      <c r="J370">
+        <v>1827.25</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>11</v>
+      </c>
+      <c r="B371" t="s">
+        <v>199</v>
+      </c>
+      <c r="C371" t="s">
+        <v>200</v>
+      </c>
+      <c r="D371" t="s">
+        <v>14</v>
+      </c>
+      <c r="E371" t="s">
+        <v>201</v>
+      </c>
+      <c r="F371" t="s">
+        <v>14</v>
+      </c>
+      <c r="G371" t="s">
+        <v>14</v>
+      </c>
+      <c r="H371" t="s">
+        <v>606</v>
+      </c>
+      <c r="I371">
+        <v>15</v>
+      </c>
+      <c r="J371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>11</v>
+      </c>
+      <c r="B372" t="s">
+        <v>203</v>
+      </c>
+      <c r="C372" t="s">
+        <v>204</v>
+      </c>
+      <c r="D372" t="s">
+        <v>14</v>
+      </c>
+      <c r="E372" t="s">
+        <v>205</v>
+      </c>
+      <c r="F372" t="s">
+        <v>14</v>
+      </c>
+      <c r="G372" t="s">
+        <v>14</v>
+      </c>
+      <c r="H372" t="s">
+        <v>607</v>
+      </c>
+      <c r="I372">
+        <v>2</v>
+      </c>
+      <c r="J372">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="373" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>11</v>
+      </c>
+      <c r="B373" t="s">
+        <v>207</v>
+      </c>
+      <c r="C373" t="s">
+        <v>208</v>
+      </c>
+      <c r="D373" t="s">
+        <v>14</v>
+      </c>
+      <c r="E373" t="s">
+        <v>209</v>
+      </c>
+      <c r="F373" t="s">
+        <v>14</v>
+      </c>
+      <c r="G373" t="s">
+        <v>14</v>
+      </c>
+      <c r="H373" t="s">
+        <v>608</v>
+      </c>
+      <c r="I373">
+        <v>12</v>
+      </c>
+      <c r="J373">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>11</v>
+      </c>
+      <c r="B374" t="s">
+        <v>211</v>
+      </c>
+      <c r="C374" t="s">
+        <v>212</v>
+      </c>
+      <c r="D374" t="s">
+        <v>14</v>
+      </c>
+      <c r="E374" t="s">
+        <v>213</v>
+      </c>
+      <c r="F374" t="s">
+        <v>14</v>
+      </c>
+      <c r="G374" t="s">
+        <v>14</v>
+      </c>
+      <c r="H374" t="s">
+        <v>609</v>
+      </c>
+      <c r="I374">
+        <v>17</v>
+      </c>
+      <c r="J374">
+        <v>3299.71</v>
+      </c>
+    </row>
+    <row r="375" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>11</v>
+      </c>
+      <c r="B375" t="s">
+        <v>215</v>
+      </c>
+      <c r="C375" t="s">
+        <v>216</v>
+      </c>
+      <c r="D375" t="s">
+        <v>14</v>
+      </c>
+      <c r="E375" t="s">
+        <v>217</v>
+      </c>
+      <c r="F375" t="s">
+        <v>14</v>
+      </c>
+      <c r="G375" t="s">
+        <v>14</v>
+      </c>
+      <c r="H375" t="s">
+        <v>610</v>
+      </c>
+      <c r="I375">
+        <v>15</v>
+      </c>
+      <c r="J375">
+        <v>3171.76</v>
+      </c>
+    </row>
+    <row r="376" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>11</v>
+      </c>
+      <c r="B376" t="s">
+        <v>223</v>
+      </c>
+      <c r="C376" t="s">
+        <v>224</v>
+      </c>
+      <c r="D376" t="s">
+        <v>14</v>
+      </c>
+      <c r="E376" t="s">
+        <v>225</v>
+      </c>
+      <c r="F376" t="s">
+        <v>14</v>
+      </c>
+      <c r="G376" t="s">
+        <v>14</v>
+      </c>
+      <c r="H376" t="s">
+        <v>611</v>
+      </c>
+      <c r="I376">
+        <v>14</v>
+      </c>
+      <c r="J376">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="377" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>11</v>
+      </c>
+      <c r="B377" t="s">
+        <v>227</v>
+      </c>
+      <c r="C377" t="s">
+        <v>228</v>
+      </c>
+      <c r="D377" t="s">
+        <v>14</v>
+      </c>
+      <c r="E377" t="s">
+        <v>229</v>
+      </c>
+      <c r="F377" t="s">
+        <v>14</v>
+      </c>
+      <c r="G377" t="s">
+        <v>14</v>
+      </c>
+      <c r="H377" t="s">
+        <v>612</v>
+      </c>
+      <c r="I377">
+        <v>8</v>
+      </c>
+      <c r="J377">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="378" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>11</v>
+      </c>
+      <c r="B378" t="s">
+        <v>231</v>
+      </c>
+      <c r="C378" t="s">
+        <v>232</v>
+      </c>
+      <c r="D378" t="s">
+        <v>14</v>
+      </c>
+      <c r="E378" t="s">
+        <v>233</v>
+      </c>
+      <c r="F378" t="s">
+        <v>14</v>
+      </c>
+      <c r="G378" t="s">
+        <v>14</v>
+      </c>
+      <c r="H378" t="s">
+        <v>613</v>
+      </c>
+      <c r="I378">
+        <v>11</v>
+      </c>
+      <c r="J378">
+        <v>4114</v>
+      </c>
+    </row>
+    <row r="379" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>11</v>
+      </c>
+      <c r="B379" t="s">
+        <v>235</v>
+      </c>
+      <c r="C379" t="s">
+        <v>236</v>
+      </c>
+      <c r="D379" t="s">
+        <v>14</v>
+      </c>
+      <c r="E379" t="s">
+        <v>237</v>
+      </c>
+      <c r="F379" t="s">
+        <v>14</v>
+      </c>
+      <c r="G379" t="s">
+        <v>14</v>
+      </c>
+      <c r="H379" t="s">
+        <v>614</v>
+      </c>
+      <c r="I379">
+        <v>14</v>
+      </c>
+      <c r="J379">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>11</v>
+      </c>
+      <c r="B380" t="s">
+        <v>239</v>
+      </c>
+      <c r="C380" t="s">
+        <v>240</v>
+      </c>
+      <c r="D380" t="s">
+        <v>14</v>
+      </c>
+      <c r="E380" t="s">
+        <v>241</v>
+      </c>
+      <c r="F380" t="s">
+        <v>14</v>
+      </c>
+      <c r="G380" t="s">
+        <v>14</v>
+      </c>
+      <c r="H380" t="s">
+        <v>615</v>
+      </c>
+      <c r="I380">
+        <v>14</v>
+      </c>
+      <c r="J380">
+        <v>3256.23</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>11</v>
+      </c>
+      <c r="B381" t="s">
+        <v>244</v>
+      </c>
+      <c r="C381" t="s">
+        <v>244</v>
+      </c>
+      <c r="D381" t="s">
+        <v>14</v>
+      </c>
+      <c r="E381" t="s">
+        <v>245</v>
+      </c>
+      <c r="F381" t="s">
+        <v>14</v>
+      </c>
+      <c r="G381" t="s">
+        <v>14</v>
+      </c>
+      <c r="H381" t="s">
+        <v>564</v>
+      </c>
+      <c r="I381">
+        <v>2</v>
+      </c>
+      <c r="J381">
+        <v>13.13</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>11</v>
+      </c>
+      <c r="B382" t="s">
+        <v>247</v>
+      </c>
+      <c r="C382" t="s">
+        <v>248</v>
+      </c>
+      <c r="D382" t="s">
+        <v>14</v>
+      </c>
+      <c r="E382" t="s">
+        <v>249</v>
+      </c>
+      <c r="F382" t="s">
+        <v>14</v>
+      </c>
+      <c r="G382" t="s">
+        <v>14</v>
+      </c>
+      <c r="H382" t="s">
+        <v>616</v>
+      </c>
+      <c r="I382">
+        <v>16</v>
+      </c>
+      <c r="J382">
+        <v>2946</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>11</v>
+      </c>
+      <c r="B383" t="s">
+        <v>251</v>
+      </c>
+      <c r="C383" t="s">
+        <v>252</v>
+      </c>
+      <c r="D383" t="s">
+        <v>14</v>
+      </c>
+      <c r="E383" t="s">
+        <v>253</v>
+      </c>
+      <c r="F383" t="s">
+        <v>14</v>
+      </c>
+      <c r="G383" t="s">
+        <v>14</v>
+      </c>
+      <c r="H383" t="s">
+        <v>617</v>
+      </c>
+      <c r="I383">
+        <v>12</v>
+      </c>
+      <c r="J383">
+        <v>3077</v>
+      </c>
+    </row>
+    <row r="384" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>11</v>
+      </c>
+      <c r="B384" t="s">
+        <v>255</v>
+      </c>
+      <c r="C384" t="s">
+        <v>256</v>
+      </c>
+      <c r="D384" t="s">
+        <v>14</v>
+      </c>
+      <c r="E384" t="s">
+        <v>257</v>
+      </c>
+      <c r="F384" t="s">
+        <v>14</v>
+      </c>
+      <c r="G384" t="s">
+        <v>14</v>
+      </c>
+      <c r="H384" t="s">
+        <v>618</v>
+      </c>
+      <c r="I384">
+        <v>18</v>
+      </c>
+      <c r="J384">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>11</v>
+      </c>
+      <c r="B385" t="s">
+        <v>259</v>
+      </c>
+      <c r="C385" t="s">
+        <v>260</v>
+      </c>
+      <c r="D385" t="s">
+        <v>14</v>
+      </c>
+      <c r="E385" t="s">
+        <v>261</v>
+      </c>
+      <c r="F385" t="s">
+        <v>14</v>
+      </c>
+      <c r="G385" t="s">
+        <v>14</v>
+      </c>
+      <c r="H385" t="s">
+        <v>619</v>
+      </c>
+      <c r="I385">
+        <v>14</v>
+      </c>
+      <c r="J385">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>11</v>
+      </c>
+      <c r="B386" t="s">
+        <v>263</v>
+      </c>
+      <c r="C386" t="s">
+        <v>264</v>
+      </c>
+      <c r="D386" t="s">
+        <v>14</v>
+      </c>
+      <c r="E386" t="s">
+        <v>265</v>
+      </c>
+      <c r="F386" t="s">
+        <v>14</v>
+      </c>
+      <c r="G386" t="s">
+        <v>14</v>
+      </c>
+      <c r="H386" t="s">
+        <v>516</v>
+      </c>
+      <c r="I386">
+        <v>1</v>
+      </c>
+      <c r="J386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>11</v>
+      </c>
+      <c r="B387" t="s">
+        <v>267</v>
+      </c>
+      <c r="C387" t="s">
+        <v>268</v>
+      </c>
+      <c r="D387" t="s">
+        <v>14</v>
+      </c>
+      <c r="E387" t="s">
+        <v>269</v>
+      </c>
+      <c r="F387" t="s">
+        <v>14</v>
+      </c>
+      <c r="G387" t="s">
+        <v>14</v>
+      </c>
+      <c r="H387" t="s">
+        <v>620</v>
+      </c>
+      <c r="I387">
+        <v>15</v>
+      </c>
+      <c r="J387">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>11</v>
+      </c>
+      <c r="B388" t="s">
+        <v>621</v>
+      </c>
+      <c r="C388" t="s">
+        <v>272</v>
+      </c>
+      <c r="D388" t="s">
+        <v>14</v>
+      </c>
+      <c r="E388" t="s">
+        <v>273</v>
+      </c>
+      <c r="F388" t="s">
+        <v>14</v>
+      </c>
+      <c r="G388" t="s">
+        <v>14</v>
+      </c>
+      <c r="H388" t="s">
+        <v>622</v>
+      </c>
+      <c r="I388">
+        <v>19</v>
+      </c>
+      <c r="J388">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="389" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>11</v>
+      </c>
+      <c r="B389" t="s">
+        <v>275</v>
+      </c>
+      <c r="C389" t="s">
+        <v>276</v>
+      </c>
+      <c r="D389" t="s">
+        <v>14</v>
+      </c>
+      <c r="E389" t="s">
+        <v>277</v>
+      </c>
+      <c r="F389" t="s">
+        <v>14</v>
+      </c>
+      <c r="G389" t="s">
+        <v>14</v>
+      </c>
+      <c r="H389" t="s">
+        <v>623</v>
+      </c>
+      <c r="I389">
+        <v>23</v>
+      </c>
+      <c r="J389">
+        <v>2298.37</v>
+      </c>
+    </row>
+    <row r="390" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>11</v>
+      </c>
+      <c r="B390" t="s">
+        <v>279</v>
+      </c>
+      <c r="C390" t="s">
+        <v>280</v>
+      </c>
+      <c r="D390" t="s">
+        <v>14</v>
+      </c>
+      <c r="E390" t="s">
+        <v>281</v>
+      </c>
+      <c r="F390" t="s">
+        <v>14</v>
+      </c>
+      <c r="G390" t="s">
+        <v>14</v>
+      </c>
+      <c r="H390" t="s">
+        <v>624</v>
+      </c>
+      <c r="I390">
+        <v>15</v>
+      </c>
+      <c r="J390">
+        <v>3015.63</v>
+      </c>
+    </row>
+    <row r="391" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>11</v>
+      </c>
+      <c r="B391" t="s">
+        <v>283</v>
+      </c>
+      <c r="C391" t="s">
+        <v>284</v>
+      </c>
+      <c r="D391" t="s">
+        <v>14</v>
+      </c>
+      <c r="E391" t="s">
+        <v>285</v>
+      </c>
+      <c r="F391" t="s">
+        <v>14</v>
+      </c>
+      <c r="G391" t="s">
+        <v>14</v>
+      </c>
+      <c r="H391" t="s">
+        <v>625</v>
+      </c>
+      <c r="I391">
+        <v>18</v>
+      </c>
+      <c r="J391">
+        <v>3173.5</v>
+      </c>
+    </row>
+    <row r="392" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>11</v>
+      </c>
+      <c r="B392" t="s">
+        <v>287</v>
+      </c>
+      <c r="C392" t="s">
+        <v>288</v>
+      </c>
+      <c r="D392" t="s">
+        <v>14</v>
+      </c>
+      <c r="E392" t="s">
+        <v>289</v>
+      </c>
+      <c r="F392" t="s">
+        <v>14</v>
+      </c>
+      <c r="G392" t="s">
+        <v>14</v>
+      </c>
+      <c r="H392" t="s">
+        <v>626</v>
+      </c>
+      <c r="I392">
+        <v>15</v>
+      </c>
+      <c r="J392">
+        <v>2604.88</v>
+      </c>
+    </row>
+    <row r="393" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>11</v>
+      </c>
+      <c r="B393" t="s">
+        <v>291</v>
+      </c>
+      <c r="C393" t="s">
+        <v>292</v>
+      </c>
+      <c r="D393" t="s">
+        <v>14</v>
+      </c>
+      <c r="E393" t="s">
+        <v>293</v>
+      </c>
+      <c r="F393" t="s">
+        <v>14</v>
+      </c>
+      <c r="G393" t="s">
+        <v>14</v>
+      </c>
+      <c r="H393" t="s">
+        <v>627</v>
+      </c>
+      <c r="I393">
+        <v>13</v>
+      </c>
+      <c r="J393">
+        <v>3129.81</v>
+      </c>
+    </row>
+    <row r="394" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>11</v>
+      </c>
+      <c r="B394" t="s">
+        <v>295</v>
+      </c>
+      <c r="C394" t="s">
+        <v>296</v>
+      </c>
+      <c r="D394" t="s">
+        <v>14</v>
+      </c>
+      <c r="E394" t="s">
+        <v>297</v>
+      </c>
+      <c r="F394" t="s">
+        <v>14</v>
+      </c>
+      <c r="G394" t="s">
+        <v>14</v>
+      </c>
+      <c r="H394" t="s">
+        <v>628</v>
+      </c>
+      <c r="I394">
+        <v>16</v>
+      </c>
+      <c r="J394">
+        <v>4715.88</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>11</v>
+      </c>
+      <c r="B395" t="s">
+        <v>299</v>
+      </c>
+      <c r="C395" t="s">
+        <v>300</v>
+      </c>
+      <c r="D395" t="s">
+        <v>14</v>
+      </c>
+      <c r="E395" t="s">
+        <v>301</v>
+      </c>
+      <c r="F395" t="s">
+        <v>14</v>
+      </c>
+      <c r="G395" t="s">
+        <v>14</v>
+      </c>
+      <c r="H395" t="s">
+        <v>629</v>
+      </c>
+      <c r="I395">
+        <v>13</v>
+      </c>
+      <c r="J395">
+        <v>2290.39</v>
+      </c>
+    </row>
+    <row r="396" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>11</v>
+      </c>
+      <c r="B396" t="s">
+        <v>303</v>
+      </c>
+      <c r="C396" t="s">
+        <v>304</v>
+      </c>
+      <c r="D396" t="s">
+        <v>14</v>
+      </c>
+      <c r="E396" t="s">
+        <v>305</v>
+      </c>
+      <c r="F396" t="s">
+        <v>14</v>
+      </c>
+      <c r="G396" t="s">
+        <v>14</v>
+      </c>
+      <c r="H396" t="s">
+        <v>630</v>
+      </c>
+      <c r="I396">
+        <v>10</v>
+      </c>
+      <c r="J396">
+        <v>4645.13</v>
+      </c>
+    </row>
+    <row r="397" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>11</v>
+      </c>
+      <c r="B397" t="s">
+        <v>307</v>
+      </c>
+      <c r="C397" t="s">
+        <v>308</v>
+      </c>
+      <c r="D397" t="s">
+        <v>14</v>
+      </c>
+      <c r="E397" t="s">
+        <v>309</v>
+      </c>
+      <c r="F397" t="s">
+        <v>14</v>
+      </c>
+      <c r="G397" t="s">
+        <v>14</v>
+      </c>
+      <c r="H397" t="s">
+        <v>631</v>
+      </c>
+      <c r="I397">
+        <v>14</v>
+      </c>
+      <c r="J397">
+        <v>3619.93</v>
+      </c>
+    </row>
+    <row r="398" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>11</v>
+      </c>
+      <c r="B398" t="s">
+        <v>315</v>
+      </c>
+      <c r="C398" t="s">
+        <v>316</v>
+      </c>
+      <c r="D398" t="s">
+        <v>14</v>
+      </c>
+      <c r="E398" t="s">
+        <v>317</v>
+      </c>
+      <c r="F398" t="s">
+        <v>14</v>
+      </c>
+      <c r="G398" t="s">
+        <v>14</v>
+      </c>
+      <c r="H398" t="s">
+        <v>632</v>
+      </c>
+      <c r="I398">
+        <v>15</v>
+      </c>
+      <c r="J398">
+        <v>2673.26</v>
+      </c>
+    </row>
+    <row r="399" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>11</v>
+      </c>
+      <c r="B399" t="s">
+        <v>319</v>
+      </c>
+      <c r="C399" t="s">
+        <v>320</v>
+      </c>
+      <c r="D399" t="s">
+        <v>14</v>
+      </c>
+      <c r="E399" t="s">
+        <v>321</v>
+      </c>
+      <c r="F399" t="s">
+        <v>14</v>
+      </c>
+      <c r="G399" t="s">
+        <v>14</v>
+      </c>
+      <c r="H399" t="s">
+        <v>633</v>
+      </c>
+      <c r="I399">
+        <v>11</v>
+      </c>
+      <c r="J399">
+        <v>3362.07</v>
+      </c>
+    </row>
+    <row r="400" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>11</v>
+      </c>
+      <c r="B400" t="s">
+        <v>323</v>
+      </c>
+      <c r="C400" t="s">
+        <v>324</v>
+      </c>
+      <c r="D400" t="s">
+        <v>14</v>
+      </c>
+      <c r="E400" t="s">
+        <v>325</v>
+      </c>
+      <c r="F400" t="s">
+        <v>14</v>
+      </c>
+      <c r="G400" t="s">
+        <v>14</v>
+      </c>
+      <c r="H400" t="s">
+        <v>634</v>
+      </c>
+      <c r="I400">
+        <v>11</v>
+      </c>
+      <c r="J400">
+        <v>3313.45</v>
+      </c>
+    </row>
+    <row r="401" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>11</v>
+      </c>
+      <c r="B401" t="s">
+        <v>327</v>
+      </c>
+      <c r="C401" t="s">
+        <v>328</v>
+      </c>
+      <c r="D401" t="s">
+        <v>14</v>
+      </c>
+      <c r="E401" t="s">
+        <v>329</v>
+      </c>
+      <c r="F401" t="s">
+        <v>14</v>
+      </c>
+      <c r="G401" t="s">
+        <v>14</v>
+      </c>
+      <c r="H401" t="s">
+        <v>623</v>
+      </c>
+      <c r="I401">
+        <v>14</v>
+      </c>
+      <c r="J401">
+        <v>2937</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>11</v>
+      </c>
+      <c r="B402" t="s">
+        <v>331</v>
+      </c>
+      <c r="C402" t="s">
+        <v>332</v>
+      </c>
+      <c r="D402" t="s">
+        <v>14</v>
+      </c>
+      <c r="E402" t="s">
+        <v>333</v>
+      </c>
+      <c r="F402" t="s">
+        <v>14</v>
+      </c>
+      <c r="G402" t="s">
+        <v>14</v>
+      </c>
+      <c r="H402" t="s">
+        <v>635</v>
+      </c>
+      <c r="I402">
+        <v>4</v>
+      </c>
+      <c r="J402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>11</v>
+      </c>
+      <c r="B403" t="s">
+        <v>335</v>
+      </c>
+      <c r="C403" t="s">
+        <v>336</v>
+      </c>
+      <c r="D403" t="s">
+        <v>14</v>
+      </c>
+      <c r="E403" t="s">
+        <v>337</v>
+      </c>
+      <c r="F403" t="s">
+        <v>14</v>
+      </c>
+      <c r="G403" t="s">
+        <v>14</v>
+      </c>
+      <c r="H403" t="s">
+        <v>636</v>
+      </c>
+      <c r="I403">
+        <v>16</v>
+      </c>
+      <c r="J403">
+        <v>3412.4</v>
+      </c>
+    </row>
+    <row r="404" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>11</v>
+      </c>
+      <c r="B404" t="s">
+        <v>339</v>
+      </c>
+      <c r="C404" t="s">
+        <v>340</v>
+      </c>
+      <c r="D404" t="s">
+        <v>14</v>
+      </c>
+      <c r="E404" t="s">
+        <v>341</v>
+      </c>
+      <c r="F404" t="s">
+        <v>14</v>
+      </c>
+      <c r="G404" t="s">
+        <v>14</v>
+      </c>
+      <c r="H404" t="s">
+        <v>637</v>
+      </c>
+      <c r="I404">
+        <v>10</v>
+      </c>
+      <c r="J404">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="405" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A405" t="s">
+        <v>11</v>
+      </c>
+      <c r="B405" t="s">
+        <v>343</v>
+      </c>
+      <c r="C405" t="s">
+        <v>344</v>
+      </c>
+      <c r="D405" t="s">
+        <v>14</v>
+      </c>
+      <c r="E405" t="s">
+        <v>345</v>
+      </c>
+      <c r="F405" t="s">
+        <v>14</v>
+      </c>
+      <c r="G405" t="s">
+        <v>14</v>
+      </c>
+      <c r="H405" t="s">
+        <v>638</v>
+      </c>
+      <c r="I405">
+        <v>16</v>
+      </c>
+      <c r="J405">
+        <v>3142.97</v>
+      </c>
+    </row>
+    <row r="406" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>11</v>
+      </c>
+      <c r="B406" t="s">
+        <v>347</v>
+      </c>
+      <c r="C406" t="s">
+        <v>348</v>
+      </c>
+      <c r="D406" t="s">
+        <v>14</v>
+      </c>
+      <c r="E406" t="s">
+        <v>349</v>
+      </c>
+      <c r="F406" t="s">
+        <v>14</v>
+      </c>
+      <c r="G406" t="s">
+        <v>14</v>
+      </c>
+      <c r="H406" t="s">
+        <v>639</v>
+      </c>
+      <c r="I406">
+        <v>6</v>
+      </c>
+      <c r="J406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>11</v>
+      </c>
+      <c r="B407" t="s">
+        <v>355</v>
+      </c>
+      <c r="C407" t="s">
+        <v>356</v>
+      </c>
+      <c r="D407" t="s">
+        <v>14</v>
+      </c>
+      <c r="E407" t="s">
+        <v>357</v>
+      </c>
+      <c r="F407" t="s">
+        <v>14</v>
+      </c>
+      <c r="G407" t="s">
+        <v>14</v>
+      </c>
+      <c r="H407" t="s">
+        <v>640</v>
+      </c>
+      <c r="I407">
+        <v>7</v>
+      </c>
+      <c r="J407">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="408" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>11</v>
+      </c>
+      <c r="B408" t="s">
+        <v>359</v>
+      </c>
+      <c r="C408" t="s">
+        <v>360</v>
+      </c>
+      <c r="D408" t="s">
+        <v>14</v>
+      </c>
+      <c r="E408" t="s">
+        <v>361</v>
+      </c>
+      <c r="F408" t="s">
+        <v>14</v>
+      </c>
+      <c r="G408" t="s">
+        <v>14</v>
+      </c>
+      <c r="H408" t="s">
+        <v>641</v>
+      </c>
+      <c r="I408">
+        <v>20</v>
+      </c>
+      <c r="J408">
+        <v>3178</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>11</v>
+      </c>
+      <c r="B409" t="s">
+        <v>363</v>
+      </c>
+      <c r="C409" t="s">
+        <v>364</v>
+      </c>
+      <c r="D409" t="s">
+        <v>14</v>
+      </c>
+      <c r="E409" t="s">
+        <v>365</v>
+      </c>
+      <c r="F409" t="s">
+        <v>14</v>
+      </c>
+      <c r="G409" t="s">
+        <v>14</v>
+      </c>
+      <c r="H409" t="s">
+        <v>642</v>
+      </c>
+      <c r="I409">
+        <v>16</v>
+      </c>
+      <c r="J409">
+        <v>2344.54</v>
+      </c>
+    </row>
+    <row r="410" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>11</v>
+      </c>
+      <c r="B410" t="s">
+        <v>367</v>
+      </c>
+      <c r="C410" t="s">
+        <v>368</v>
+      </c>
+      <c r="D410" t="s">
+        <v>14</v>
+      </c>
+      <c r="E410" t="s">
+        <v>369</v>
+      </c>
+      <c r="F410" t="s">
+        <v>14</v>
+      </c>
+      <c r="G410" t="s">
+        <v>14</v>
+      </c>
+      <c r="H410" t="s">
+        <v>643</v>
+      </c>
+      <c r="I410">
+        <v>15</v>
+      </c>
+      <c r="J410">
+        <v>2634.48</v>
+      </c>
+    </row>
+    <row r="411" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>11</v>
+      </c>
+      <c r="B411" t="s">
+        <v>644</v>
+      </c>
+      <c r="C411" t="s">
+        <v>372</v>
+      </c>
+      <c r="D411" t="s">
+        <v>14</v>
+      </c>
+      <c r="E411" t="s">
+        <v>373</v>
+      </c>
+      <c r="F411" t="s">
+        <v>14</v>
+      </c>
+      <c r="G411" t="s">
+        <v>14</v>
+      </c>
+      <c r="H411" t="s">
+        <v>645</v>
+      </c>
+      <c r="I411">
+        <v>5</v>
+      </c>
+      <c r="J411">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="412" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>11</v>
+      </c>
+      <c r="B412" t="s">
+        <v>219</v>
+      </c>
+      <c r="C412" t="s">
+        <v>376</v>
+      </c>
+      <c r="D412" t="s">
+        <v>14</v>
+      </c>
+      <c r="E412" t="s">
+        <v>377</v>
+      </c>
+      <c r="F412" t="s">
+        <v>14</v>
+      </c>
+      <c r="G412" t="s">
+        <v>14</v>
+      </c>
+      <c r="H412" t="s">
+        <v>646</v>
+      </c>
+      <c r="I412">
+        <v>13</v>
+      </c>
+      <c r="J412">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="413" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>11</v>
+      </c>
+      <c r="B413" t="s">
+        <v>647</v>
+      </c>
+      <c r="C413" t="s">
+        <v>648</v>
+      </c>
+      <c r="D413" t="s">
+        <v>14</v>
+      </c>
+      <c r="E413" t="s">
+        <v>649</v>
+      </c>
+      <c r="F413" t="s">
+        <v>14</v>
+      </c>
+      <c r="G413" t="s">
+        <v>14</v>
+      </c>
+      <c r="H413" t="s">
+        <v>611</v>
+      </c>
+      <c r="I413">
+        <v>13</v>
+      </c>
+      <c r="J413">
+        <v>3105.94</v>
+      </c>
+    </row>
+    <row r="414" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>11</v>
+      </c>
+      <c r="B414" t="s">
+        <v>379</v>
+      </c>
+      <c r="C414" t="s">
+        <v>380</v>
+      </c>
+      <c r="D414" t="s">
+        <v>14</v>
+      </c>
+      <c r="E414" t="s">
+        <v>381</v>
+      </c>
+      <c r="F414" t="s">
+        <v>14</v>
+      </c>
+      <c r="G414" t="s">
+        <v>14</v>
+      </c>
+      <c r="H414" t="s">
+        <v>650</v>
+      </c>
+      <c r="I414">
+        <v>21</v>
+      </c>
+      <c r="J414">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="415" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>11</v>
+      </c>
+      <c r="B415" t="s">
+        <v>383</v>
+      </c>
+      <c r="C415" t="s">
+        <v>384</v>
+      </c>
+      <c r="D415" t="s">
+        <v>14</v>
+      </c>
+      <c r="E415" t="s">
+        <v>385</v>
+      </c>
+      <c r="F415" t="s">
+        <v>14</v>
+      </c>
+      <c r="G415" t="s">
+        <v>14</v>
+      </c>
+      <c r="H415" t="s">
+        <v>651</v>
+      </c>
+      <c r="I415">
+        <v>14</v>
+      </c>
+      <c r="J415">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="416" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>11</v>
+      </c>
+      <c r="B416" t="s">
+        <v>387</v>
+      </c>
+      <c r="C416" t="s">
+        <v>388</v>
+      </c>
+      <c r="D416" t="s">
+        <v>14</v>
+      </c>
+      <c r="E416" t="s">
+        <v>389</v>
+      </c>
+      <c r="F416" t="s">
+        <v>14</v>
+      </c>
+      <c r="G416" t="s">
+        <v>14</v>
+      </c>
+      <c r="H416" t="s">
+        <v>652</v>
+      </c>
+      <c r="I416">
+        <v>16</v>
+      </c>
+      <c r="J416">
+        <v>2885.75</v>
+      </c>
+    </row>
+    <row r="417" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>11</v>
+      </c>
+      <c r="B417" t="s">
+        <v>391</v>
+      </c>
+      <c r="C417" t="s">
+        <v>392</v>
+      </c>
+      <c r="D417" t="s">
+        <v>14</v>
+      </c>
+      <c r="E417" t="s">
+        <v>393</v>
+      </c>
+      <c r="F417" t="s">
+        <v>14</v>
+      </c>
+      <c r="G417" t="s">
+        <v>14</v>
+      </c>
+      <c r="H417" t="s">
+        <v>653</v>
+      </c>
+      <c r="I417">
+        <v>13</v>
+      </c>
+      <c r="J417">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="418" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>11</v>
+      </c>
+      <c r="B418" t="s">
+        <v>395</v>
+      </c>
+      <c r="C418" t="s">
+        <v>396</v>
+      </c>
+      <c r="D418" t="s">
+        <v>14</v>
+      </c>
+      <c r="E418" t="s">
+        <v>397</v>
+      </c>
+      <c r="F418" t="s">
+        <v>14</v>
+      </c>
+      <c r="G418" t="s">
+        <v>14</v>
+      </c>
+      <c r="H418" t="s">
+        <v>654</v>
+      </c>
+      <c r="I418">
+        <v>24</v>
+      </c>
+      <c r="J418">
+        <v>3122.79</v>
+      </c>
+    </row>
+    <row r="419" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>11</v>
+      </c>
+      <c r="B419" t="s">
+        <v>399</v>
+      </c>
+      <c r="C419" t="s">
+        <v>400</v>
+      </c>
+      <c r="D419" t="s">
+        <v>14</v>
+      </c>
+      <c r="E419" t="s">
+        <v>401</v>
+      </c>
+      <c r="F419" t="s">
+        <v>14</v>
+      </c>
+      <c r="G419" t="s">
+        <v>14</v>
+      </c>
+      <c r="H419" t="s">
+        <v>655</v>
+      </c>
+      <c r="I419">
+        <v>14</v>
+      </c>
+      <c r="J419">
+        <v>3143.64</v>
+      </c>
+    </row>
+    <row r="420" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>11</v>
+      </c>
+      <c r="B420" t="s">
+        <v>403</v>
+      </c>
+      <c r="C420" t="s">
+        <v>404</v>
+      </c>
+      <c r="D420" t="s">
+        <v>14</v>
+      </c>
+      <c r="E420" t="s">
+        <v>405</v>
+      </c>
+      <c r="F420" t="s">
+        <v>14</v>
+      </c>
+      <c r="G420" t="s">
+        <v>14</v>
+      </c>
+      <c r="H420" t="s">
+        <v>656</v>
+      </c>
+      <c r="I420">
+        <v>14</v>
+      </c>
+      <c r="J420">
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="421" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>11</v>
+      </c>
+      <c r="B421" t="s">
+        <v>408</v>
+      </c>
+      <c r="C421" t="s">
+        <v>408</v>
+      </c>
+      <c r="D421" t="s">
+        <v>14</v>
+      </c>
+      <c r="E421" t="s">
+        <v>409</v>
+      </c>
+      <c r="F421" t="s">
+        <v>14</v>
+      </c>
+      <c r="G421" t="s">
+        <v>14</v>
+      </c>
+      <c r="H421" t="s">
+        <v>657</v>
+      </c>
+      <c r="I421">
+        <v>9</v>
+      </c>
+      <c r="J421">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="422" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>11</v>
+      </c>
+      <c r="B422" t="s">
+        <v>411</v>
+      </c>
+      <c r="C422" t="s">
+        <v>412</v>
+      </c>
+      <c r="D422" t="s">
+        <v>14</v>
+      </c>
+      <c r="E422" t="s">
+        <v>413</v>
+      </c>
+      <c r="F422" t="s">
+        <v>14</v>
+      </c>
+      <c r="G422" t="s">
+        <v>14</v>
+      </c>
+      <c r="H422" t="s">
+        <v>658</v>
+      </c>
+      <c r="I422">
+        <v>14</v>
+      </c>
+      <c r="J422">
+        <v>1446.38</v>
+      </c>
+    </row>
+    <row r="423" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>11</v>
+      </c>
+      <c r="B423" t="s">
+        <v>415</v>
+      </c>
+      <c r="C423" t="s">
+        <v>416</v>
+      </c>
+      <c r="D423" t="s">
+        <v>14</v>
+      </c>
+      <c r="E423" t="s">
+        <v>417</v>
+      </c>
+      <c r="F423" t="s">
+        <v>14</v>
+      </c>
+      <c r="G423" t="s">
+        <v>14</v>
+      </c>
+      <c r="H423" t="s">
+        <v>659</v>
+      </c>
+      <c r="I423">
+        <v>14</v>
+      </c>
+      <c r="J423">
+        <v>2472.94</v>
+      </c>
+    </row>
+    <row r="424" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>11</v>
+      </c>
+      <c r="B424" t="s">
+        <v>419</v>
+      </c>
+      <c r="C424" t="s">
+        <v>420</v>
+      </c>
+      <c r="D424" t="s">
+        <v>14</v>
+      </c>
+      <c r="E424" t="s">
+        <v>421</v>
+      </c>
+      <c r="F424" t="s">
+        <v>14</v>
+      </c>
+      <c r="G424" t="s">
+        <v>14</v>
+      </c>
+      <c r="H424" t="s">
+        <v>660</v>
+      </c>
+      <c r="I424">
+        <v>16</v>
+      </c>
+      <c r="J424">
+        <v>3595</v>
+      </c>
+    </row>
+    <row r="425" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>11</v>
+      </c>
+      <c r="B425" t="s">
+        <v>423</v>
+      </c>
+      <c r="C425" t="s">
+        <v>424</v>
+      </c>
+      <c r="D425" t="s">
+        <v>14</v>
+      </c>
+      <c r="E425" t="s">
+        <v>425</v>
+      </c>
+      <c r="F425" t="s">
+        <v>14</v>
+      </c>
+      <c r="G425" t="s">
+        <v>14</v>
+      </c>
+      <c r="H425" t="s">
+        <v>661</v>
+      </c>
+      <c r="I425">
+        <v>19</v>
+      </c>
+      <c r="J425">
+        <v>3140.27</v>
+      </c>
+    </row>
+    <row r="426" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>11</v>
+      </c>
+      <c r="B426" t="s">
+        <v>427</v>
+      </c>
+      <c r="C426" t="s">
+        <v>428</v>
+      </c>
+      <c r="D426" t="s">
+        <v>14</v>
+      </c>
+      <c r="E426" t="s">
+        <v>429</v>
+      </c>
+      <c r="F426" t="s">
+        <v>14</v>
+      </c>
+      <c r="G426" t="s">
+        <v>14</v>
+      </c>
+      <c r="H426" t="s">
+        <v>662</v>
+      </c>
+      <c r="I426">
+        <v>14</v>
+      </c>
+      <c r="J426">
+        <v>4094.94</v>
+      </c>
+    </row>
+    <row r="427" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>11</v>
+      </c>
+      <c r="B427" t="s">
+        <v>431</v>
+      </c>
+      <c r="C427" t="s">
+        <v>432</v>
+      </c>
+      <c r="D427" t="s">
+        <v>14</v>
+      </c>
+      <c r="E427" t="s">
+        <v>433</v>
+      </c>
+      <c r="F427" t="s">
+        <v>14</v>
+      </c>
+      <c r="G427" t="s">
+        <v>14</v>
+      </c>
+      <c r="H427" t="s">
+        <v>663</v>
+      </c>
+      <c r="I427">
+        <v>20</v>
+      </c>
+      <c r="J427">
+        <v>2374.09</v>
+      </c>
+    </row>
+    <row r="428" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>11</v>
+      </c>
+      <c r="B428" t="s">
+        <v>435</v>
+      </c>
+      <c r="C428" t="s">
+        <v>436</v>
+      </c>
+      <c r="D428" t="s">
+        <v>14</v>
+      </c>
+      <c r="E428" t="s">
+        <v>437</v>
+      </c>
+      <c r="F428" t="s">
+        <v>14</v>
+      </c>
+      <c r="G428" t="s">
+        <v>14</v>
+      </c>
+      <c r="H428" t="s">
+        <v>664</v>
+      </c>
+      <c r="I428">
+        <v>10</v>
+      </c>
+      <c r="J428">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="429" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>11</v>
+      </c>
+      <c r="B429" t="s">
+        <v>439</v>
+      </c>
+      <c r="C429" t="s">
+        <v>440</v>
+      </c>
+      <c r="D429" t="s">
+        <v>14</v>
+      </c>
+      <c r="E429" t="s">
+        <v>441</v>
+      </c>
+      <c r="F429" t="s">
+        <v>14</v>
+      </c>
+      <c r="G429" t="s">
+        <v>14</v>
+      </c>
+      <c r="H429" t="s">
+        <v>665</v>
+      </c>
+      <c r="I429">
+        <v>26</v>
+      </c>
+      <c r="J429">
+        <v>3347.6</v>
+      </c>
+    </row>
+    <row r="430" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>11</v>
+      </c>
+      <c r="B430" t="s">
+        <v>443</v>
+      </c>
+      <c r="C430" t="s">
+        <v>444</v>
+      </c>
+      <c r="D430" t="s">
+        <v>14</v>
+      </c>
+      <c r="E430" t="s">
+        <v>445</v>
+      </c>
+      <c r="F430" t="s">
+        <v>14</v>
+      </c>
+      <c r="G430" t="s">
+        <v>14</v>
+      </c>
+      <c r="H430" t="s">
+        <v>666</v>
+      </c>
+      <c r="I430">
+        <v>14</v>
+      </c>
+      <c r="J430">
+        <v>3396.79</v>
+      </c>
+    </row>
+    <row r="431" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>11</v>
+      </c>
+      <c r="B431" t="s">
+        <v>447</v>
+      </c>
+      <c r="C431" t="s">
+        <v>448</v>
+      </c>
+      <c r="D431" t="s">
+        <v>14</v>
+      </c>
+      <c r="E431" t="s">
+        <v>449</v>
+      </c>
+      <c r="F431" t="s">
+        <v>14</v>
+      </c>
+      <c r="G431" t="s">
+        <v>14</v>
+      </c>
+      <c r="H431" t="s">
+        <v>667</v>
+      </c>
+      <c r="I431">
+        <v>11</v>
+      </c>
+      <c r="J431">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="432" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>11</v>
+      </c>
+      <c r="B432" t="s">
+        <v>451</v>
+      </c>
+      <c r="C432" t="s">
+        <v>452</v>
+      </c>
+      <c r="D432" t="s">
+        <v>14</v>
+      </c>
+      <c r="E432" t="s">
+        <v>453</v>
+      </c>
+      <c r="F432" t="s">
+        <v>14</v>
+      </c>
+      <c r="G432" t="s">
+        <v>14</v>
+      </c>
+      <c r="H432" t="s">
+        <v>668</v>
+      </c>
+      <c r="I432">
+        <v>25</v>
+      </c>
+      <c r="J432">
+        <v>3351.75</v>
+      </c>
+    </row>
+    <row r="433" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>11</v>
+      </c>
+      <c r="B433" t="s">
+        <v>455</v>
+      </c>
+      <c r="C433" t="s">
+        <v>456</v>
+      </c>
+      <c r="D433" t="s">
+        <v>14</v>
+      </c>
+      <c r="E433" t="s">
+        <v>457</v>
+      </c>
+      <c r="F433" t="s">
+        <v>14</v>
+      </c>
+      <c r="G433" t="s">
+        <v>14</v>
+      </c>
+      <c r="H433" t="s">
+        <v>669</v>
+      </c>
+      <c r="I433">
+        <v>3</v>
+      </c>
+      <c r="J433">
+        <v>441.19</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K215">
     <sortCondition ref="A1:A215"/>
   </sortState>
-  <conditionalFormatting sqref="C325:C1048576 C1:C215">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="C1:C324 C434:C1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C216:C324">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C434:C1048576 C1:C215">
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C325:C433">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C325:C433">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>